<commit_message>
rebuilding site Tue 13 Oct 2020 07:09:32 PM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/EndReaction.xlsx
+++ b/engineering/courses/mae101/docs/EndReaction.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
   <si>
     <t xml:space="preserve">End Reaction of a Loaded Beam</t>
   </si>
@@ -39,7 +39,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Theoretical R</t>
+      <t xml:space="preserve"> R</t>
     </r>
     <r>
       <rPr>
@@ -62,7 +62,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Theoretical R</t>
+      <t xml:space="preserve">R</t>
     </r>
     <r>
       <rPr>
@@ -77,10 +77,56 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Distance of (A)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance of (B)</t>
+    <t xml:space="preserve">Distance (a)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance (b)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F497D"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color rgb="FF1F497D"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F497D"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color rgb="FF1F497D"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">EXPERIMENTAL DATA 3:</t>
@@ -104,6 +150,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,6 +172,7 @@
       <sz val="14"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -240,7 +288,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,23 +396,65 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>447480</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>402840</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>93960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4728960" y="3765240"/>
+          <a:ext cx="4618440" cy="1394640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:K23"/>
+  <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M10" activeCellId="0" sqref="M10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.14"/>
@@ -379,352 +469,354 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
+    <row r="6" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="H6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J5" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="K5" s="6" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5" t="n">
-        <v>2.49</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>1.51</v>
-      </c>
-      <c r="D6" s="6" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>2.51</v>
-      </c>
-      <c r="I6" s="6" t="n">
-        <v>1.49</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="K6" s="6" t="n">
-        <v>22.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="n">
-        <v>2.795</v>
+        <v>2</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>1.215</v>
+        <v>2</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>2.795</v>
+        <v>2</v>
       </c>
       <c r="I7" s="6" t="n">
-        <v>1.21</v>
-      </c>
-      <c r="J7" s="5" t="n">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>18</v>
       </c>
       <c r="K7" s="6" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="K8" s="6" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="5" t="n">
+        <v>2.795</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>1.215</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>2.795</v>
+      </c>
+      <c r="I9" s="6" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K9" s="6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="5" t="n">
         <v>3.335</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C10" s="6" t="n">
         <v>0.68</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D10" s="6" t="n">
         <v>6.125</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E10" s="6" t="n">
         <v>29.93</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H10" s="5" t="n">
         <v>3.255</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I10" s="6" t="n">
         <v>0.75</v>
       </c>
-      <c r="J8" s="5" t="n">
+      <c r="J10" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K8" s="6" t="n">
+      <c r="K10" s="6" t="n">
         <v>29</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="s">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I13" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="E12" s="6" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="H12" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I12" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J12" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="K12" s="6" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5" t="n">
-        <v>3.22</v>
-      </c>
-      <c r="C13" s="6" t="n">
-        <v>1.88</v>
-      </c>
-      <c r="D13" s="6" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="E13" s="6" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <v>2.51</v>
-      </c>
-      <c r="I13" s="6" t="n">
-        <v>1.49</v>
-      </c>
-      <c r="J13" s="5" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="K13" s="6" t="n">
-        <v>22.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5" t="n">
-        <v>3.73</v>
+        <v>2</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>1.22</v>
+        <v>2</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>8.5</v>
+        <v>16.5</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>24.5</v>
+        <v>16.5</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>2.795</v>
+        <v>2</v>
       </c>
       <c r="I14" s="6" t="n">
-        <v>1.21</v>
-      </c>
-      <c r="J14" s="5" t="n">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="J14" s="6" t="n">
+        <v>18</v>
       </c>
       <c r="K14" s="6" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="I15" s="6" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="J15" s="5" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="5" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="C16" s="6" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>2.795</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K16" s="6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="5" t="n">
         <v>4.33</v>
       </c>
-      <c r="C15" s="6" t="n">
+      <c r="C17" s="6" t="n">
         <v>0.66</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D17" s="6" t="n">
         <v>4.5</v>
       </c>
-      <c r="E15" s="6" t="n">
+      <c r="E17" s="6" t="n">
         <v>25.5</v>
       </c>
-      <c r="H15" s="5" t="n">
+      <c r="H17" s="5" t="n">
         <v>3.255</v>
       </c>
-      <c r="I15" s="6" t="n">
+      <c r="I17" s="6" t="n">
         <v>0.75</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J17" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K15" s="6" t="n">
+      <c r="K17" s="6" t="n">
         <v>29</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="3" t="s">
+    <row r="20" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5" t="n">
+    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="6" t="n">
+      <c r="C22" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="6" t="n">
+      <c r="D22" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="E20" s="6" t="n">
+      <c r="E22" s="6" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5" t="n">
+    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="5" t="n">
         <v>0.67</v>
       </c>
-      <c r="C21" s="6" t="n">
+      <c r="C23" s="6" t="n">
         <v>1.33</v>
       </c>
-      <c r="D21" s="6" t="n">
+      <c r="D23" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="E21" s="6" t="n">
+      <c r="E23" s="6" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="8" t="n">
+    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="8" t="n">
         <v>0.32</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C24" s="9" t="n">
         <v>1.68</v>
       </c>
-      <c r="D22" s="9" t="n">
+      <c r="D24" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="E22" s="9" t="n">
+      <c r="E24" s="9" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -737,5 +829,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>